<commit_message>
Fix handling of nested loops
The problem was that in loops offsets would have to be calculated
so the same row in each iteration would not simply be overwritten
each time.
To accomplish this, multiple mechanisms have been introduced:
* Keep track of the depth of the loop
* Keep track of how many placeholders were already substituted in
    this loop iteration
* Calculate the size of a loop iteration where all placeholders have
    been substituted
* Calculate the size of a loop with placeholders not substituted
With this information, the offsets could be added and subtracted correctly:
* The replaced size is added to the offset each iteration
* The unreplaced size is removed from the offset after each loop
* When the generate function iterated through all placeholders, readd the
     offset so we do not substract it multiple times

Signed-off-by: Anton Oellerer <a.oellerer@docu-tools.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/excel/NestedLoopDocument.xlsx
+++ b/src/test/resources/templates/excel/NestedLoopDocument.xlsx
@@ -20,38 +20,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t xml:space="preserve">This is the rythm of the night</t>
   </si>
   <si>
-    <t xml:space="preserve">The night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ooh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oh yeah</t>
-  </si>
-  <si>
     <t xml:space="preserve">{{services}}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{shipName}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/services}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{visitedPlanets}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{planetName}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/visitedPlanets}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ship Name:</t>
   </si>
   <si>
-    <t xml:space="preserve">{{shipName}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{visitedPlanets}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Planet Name:</t>
   </si>
   <si>
-    <t xml:space="preserve">{{planetName}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{{visitedCities}}</t>
   </si>
   <si>
@@ -64,10 +61,7 @@
     <t xml:space="preserve">{{/visitedCities}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{/visitedPlanets}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{/services}}</t>
+    <t xml:space="preserve">--------------------</t>
   </si>
   <si>
     <t xml:space="preserve">Das Denken der Gedanken ist ein gedankeloses Denken</t>
@@ -81,7 +75,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,13 +96,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -160,24 +147,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -198,99 +181,184 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="2" t="n">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="2" t="n">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="3" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="0" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="3" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="0" t="s">
+      <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="0" t="s">
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="0" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="0" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>